<commit_message>
formatting added to excel export
</commit_message>
<xml_diff>
--- a/Export.xlsx
+++ b/Export.xlsx
@@ -20,27 +20,45 @@
     <t>Test Script Export</t>
   </si>
   <si>
+    <t>Test Export</t>
+  </si>
+  <si>
+    <t>Default - Default - Default Script Overview</t>
+  </si>
+  <si>
+    <t>Workflow Name</t>
+  </si>
+  <si>
+    <t>Action Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Start HDRP Engine Run</t>
+  </si>
+  <si>
+    <t>Start an Engine Run</t>
+  </si>
+  <si>
+    <t>Start Fleet Engine Run</t>
+  </si>
+  <si>
+    <t>Allocate GL Codes</t>
+  </si>
+  <si>
+    <t>Allocate costs to GL Codes</t>
+  </si>
+  <si>
     <t>Test</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>Start HDRP Engine Run</t>
-  </si>
-  <si>
-    <t>Start an Engine Run</t>
-  </si>
-  <si>
-    <t>Start Fleet Engine Run</t>
-  </si>
-  <si>
-    <t>Allocate GL Codes</t>
-  </si>
-  <si>
-    <t>Allocate costs to GL Codes</t>
-  </si>
-  <si>
     <t>Promote a Shipment</t>
   </si>
   <si>
@@ -69,24 +87,6 @@
   </si>
   <si>
     <t>Update an Appointment against a Shipment &amp; Update the Carrier</t>
-  </si>
-  <si>
-    <t>Default - Default - Default Script Overview</t>
-  </si>
-  <si>
-    <t>Workflow Name</t>
-  </si>
-  <si>
-    <t>Action Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
   </si>
 </sst>
 </file>
@@ -94,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -102,16 +102,35 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,12 +138,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal>
+        <color rgb="FF000000"/>
+      </diagonal>
+      <vertical>
+        <color rgb="FF000000"/>
+      </vertical>
+      <horizontal>
+        <color rgb="FF000000"/>
+      </horizontal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -432,12 +480,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -465,169 +513,181 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s"/>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s"/>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s"/>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="n"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s"/>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s"/>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s"/>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>